<commit_message>
Both models and graphics implemented
</commit_message>
<xml_diff>
--- a/CharacteristicsDependancy.xlsx
+++ b/CharacteristicsDependancy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Imitation_Model\magistrature\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -66,6 +66,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -9538,10 +9539,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12" customWidth="1" collapsed="1"/>
-    <col min="8" max="15" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
+    <col min="2" max="6" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="8" max="15" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9553,93 +9554,93 @@
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>0.01</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>0.05</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>0.1</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>0.5</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2">
-        <v>5</v>
-      </c>
-      <c r="K2">
-        <v>6</v>
-      </c>
-      <c r="L2">
-        <v>7</v>
-      </c>
-      <c r="M2">
-        <v>8</v>
-      </c>
-      <c r="N2">
-        <v>9</v>
-      </c>
-      <c r="O2">
-        <v>10</v>
+      <c r="F2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>10.0</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>5.0001252531375915E-8</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>2.5003131642238185E-7</v>
       </c>
-      <c r="D3">
-        <v>5.0012528138298648E-7</v>
-      </c>
-      <c r="E3">
+      <c r="D3" t="n">
+        <v>5.001252813829865E-7</v>
+      </c>
+      <c r="E3" t="n">
         <v>2.5031351768089532E-6</v>
       </c>
-      <c r="F3">
-        <v>5.0125564539170627E-6</v>
-      </c>
-      <c r="G3">
+      <c r="F3" t="n">
+        <v>5.012556453917063E-6</v>
+      </c>
+      <c r="G3" t="n">
         <v>1.0050352264846886E-5</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="n">
         <v>1.5113578542748758E-5</v>
       </c>
-      <c r="I3">
-        <v>2.0202428331885491E-5</v>
-      </c>
-      <c r="J3">
+      <c r="I3" t="n">
+        <v>2.020242833188549E-5</v>
+      </c>
+      <c r="J3" t="n">
         <v>2.5317096635357866E-5</v>
       </c>
-      <c r="K3">
-        <v>3.0457780440013399E-5</v>
-      </c>
-      <c r="L3">
-        <v>3.5624678741736348E-5</v>
-      </c>
-      <c r="M3">
+      <c r="K3" t="n">
+        <v>3.04577804400134E-5</v>
+      </c>
+      <c r="L3" t="n">
+        <v>3.562467874173635E-5</v>
+      </c>
+      <c r="M3" t="n">
         <v>4.0817992571125354E-5</v>
       </c>
-      <c r="N3">
-        <v>4.6037925019566133E-5</v>
-      </c>
-      <c r="O3">
+      <c r="N3" t="n">
+        <v>4.603792501956613E-5</v>
+      </c>
+      <c r="O3" t="n">
         <v>5.128468126570593E-5</v>
       </c>
     </row>
@@ -9647,93 +9648,93 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>2.5000626265687957E-5</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>1.2501565821119098E-4</v>
       </c>
-      <c r="D4">
-        <v>2.5006264069149319E-4</v>
-      </c>
-      <c r="E4">
-        <v>1.2515675884044765E-3</v>
-      </c>
-      <c r="F4">
-        <v>2.5062782269585312E-3</v>
-      </c>
-      <c r="G4">
-        <v>5.0251761324234413E-3</v>
-      </c>
-      <c r="H4">
-        <v>7.55678927137438E-3</v>
-      </c>
-      <c r="I4">
-        <v>1.0101214165942743E-2</v>
-      </c>
-      <c r="J4">
-        <v>1.2658548317678932E-2</v>
-      </c>
-      <c r="K4">
-        <v>1.5228890220006699E-2</v>
-      </c>
-      <c r="L4">
-        <v>1.7812339370868176E-2</v>
-      </c>
-      <c r="M4">
-        <v>2.040899628556268E-2</v>
-      </c>
-      <c r="N4">
-        <v>2.3018962509783067E-2</v>
-      </c>
-      <c r="O4">
-        <v>2.5642340632852964E-2</v>
+      <c r="D4" t="n">
+        <v>2.500626406914932E-4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0012515675884044765</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.002506278226958531</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.005025176132423441</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.00755678927137438</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.010101214165942743</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.012658548317678932</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.015228890220006699</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.017812339370868176</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.02040899628556268</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.023018962509783067</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.025642340632852964</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>4.003204164613357E-4</v>
       </c>
-      <c r="C5">
-        <v>2.0080361607151824E-3</v>
-      </c>
-      <c r="D5">
-        <v>4.0322743236867881E-3</v>
-      </c>
-      <c r="E5">
-        <v>2.083376737015355E-2</v>
-      </c>
-      <c r="F5">
-        <v>4.348015131092655E-2</v>
-      </c>
-      <c r="G5">
-        <v>9.524716639679949E-2</v>
-      </c>
-      <c r="H5">
+      <c r="C5" t="n">
+        <v>0.0020080361607151824</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.004032274323686788</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.02083376737015355</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.04348015131092655</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.09524716639679949</v>
+      </c>
+      <c r="H5" t="n">
         <v>0.15791967152604458</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="n">
         <v>0.23534949355873</v>
       </c>
-      <c r="J5">
+      <c r="J5" t="n">
         <v>0.33344443336836815</v>
       </c>
-      <c r="K5">
+      <c r="K5" t="n">
         <v>0.46174933739884616</v>
       </c>
-      <c r="L5">
-        <v>0.63671090175780365</v>
-      </c>
-      <c r="M5">
-        <v>0.88870101485615294</v>
-      </c>
-      <c r="N5">
+      <c r="L5" t="n">
+        <v>0.6367109017578036</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.8887010148561529</v>
+      </c>
+      <c r="N5" t="n">
         <v>1.2753533373396806</v>
       </c>
-      <c r="O5">
+      <c r="O5" t="n">
         <v>1.8875107776524573</v>
       </c>
     </row>
@@ -9741,46 +9742,46 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>4.0072073687779693E-4</v>
-      </c>
-      <c r="C6">
-        <v>2.0100441968758979E-3</v>
-      </c>
-      <c r="D6">
-        <v>4.0363065980104744E-3</v>
-      </c>
-      <c r="E6">
-        <v>2.0854601137523701E-2</v>
-      </c>
-      <c r="F6">
-        <v>4.3523631462237485E-2</v>
-      </c>
-      <c r="G6">
-        <v>9.5342413563196296E-2</v>
-      </c>
-      <c r="H6">
+      <c r="B6" t="n">
+        <v>4.007207368777969E-4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.002010044196875898</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.004036306598010474</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0208546011375237</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.043523631462237485</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0953424135631963</v>
+      </c>
+      <c r="H6" t="n">
         <v>0.15807759119757064</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="n">
         <v>0.23558484305228874</v>
       </c>
-      <c r="J6">
-        <v>0.33377787780173651</v>
-      </c>
-      <c r="K6">
+      <c r="J6" t="n">
+        <v>0.3337778778017365</v>
+      </c>
+      <c r="K6" t="n">
         <v>0.462211086736245</v>
       </c>
-      <c r="L6">
-        <v>0.63734761265956141</v>
-      </c>
-      <c r="M6">
+      <c r="L6" t="n">
+        <v>0.6373476126595614</v>
+      </c>
+      <c r="M6" t="n">
         <v>0.8895897158710091</v>
       </c>
-      <c r="N6">
+      <c r="N6" t="n">
         <v>1.2766286906770201</v>
       </c>
-      <c r="O6">
+      <c r="O6" t="n">
         <v>1.8893982884301097</v>
       </c>
     </row>
@@ -9788,140 +9789,140 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>8.2614178210988333E-4</v>
-      </c>
-      <c r="C7">
-        <v>4.1435960784351163E-3</v>
-      </c>
-      <c r="D7">
-        <v>8.3196438129515219E-3</v>
-      </c>
-      <c r="E7">
-        <v>4.2944942366435347E-2</v>
-      </c>
-      <c r="F7">
-        <v>8.9520086113030403E-2</v>
-      </c>
-      <c r="G7">
+      <c r="B7" t="n">
+        <v>8.261417821098833E-4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.004143596078435116</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.008319643812951522</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.04294494236643535</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0895200861130304</v>
+      </c>
+      <c r="G7" t="n">
         <v>0.19563485679694892</v>
       </c>
-      <c r="H7">
+      <c r="H7" t="n">
         <v>0.3235842791520751</v>
       </c>
-      <c r="I7">
+      <c r="I7" t="n">
         <v>0.48107595563362526</v>
       </c>
-      <c r="J7">
-        <v>0.67993149368105432</v>
-      </c>
-      <c r="K7">
-        <v>0.93925022991597784</v>
-      </c>
-      <c r="L7">
+      <c r="J7" t="n">
+        <v>0.6799314936810543</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.9392502299159778</v>
+      </c>
+      <c r="L7" t="n">
         <v>1.2919421031457168</v>
       </c>
-      <c r="M7">
-        <v>1.7987813629978671</v>
-      </c>
-      <c r="N7">
-        <v>2.5750930663765228</v>
-      </c>
-      <c r="O7">
-        <v>3.8026539760779512</v>
+      <c r="M7" t="n">
+        <v>1.798781362997867</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2.575093066376523</v>
+      </c>
+      <c r="O7" t="n">
+        <v>3.802653976077951</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
-        <v>5.0001252531375918E-6</v>
-      </c>
-      <c r="C8">
-        <v>5.0006263284476364E-6</v>
-      </c>
-      <c r="D8">
-        <v>5.0012528138298641E-6</v>
-      </c>
-      <c r="E8">
+      <c r="B8" t="n">
+        <v>5.000125253137592E-6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5.000626328447636E-6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5.001252813829864E-6</v>
+      </c>
+      <c r="E8" t="n">
         <v>5.0062703536179065E-6</v>
       </c>
-      <c r="F8">
-        <v>5.0125564539170627E-6</v>
-      </c>
-      <c r="G8">
-        <v>5.0251761324234428E-6</v>
-      </c>
-      <c r="H8">
-        <v>5.0378595142495858E-6</v>
-      </c>
-      <c r="I8">
-        <v>5.0506070829713728E-6</v>
-      </c>
-      <c r="J8">
+      <c r="F8" t="n">
+        <v>5.012556453917063E-6</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5.025176132423443E-6</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5.037859514249586E-6</v>
+      </c>
+      <c r="I8" t="n">
+        <v>5.050607082971373E-6</v>
+      </c>
+      <c r="J8" t="n">
         <v>5.0634193270715734E-6</v>
       </c>
-      <c r="K8">
-        <v>5.0762967400022332E-6</v>
-      </c>
-      <c r="L8">
-        <v>5.0892398202480497E-6</v>
-      </c>
-      <c r="M8">
-        <v>5.1022490713906692E-6</v>
-      </c>
-      <c r="N8">
-        <v>5.1153250021740151E-6</v>
-      </c>
-      <c r="O8">
-        <v>5.1284681265705926E-6</v>
+      <c r="K8" t="n">
+        <v>5.076296740002233E-6</v>
+      </c>
+      <c r="L8" t="n">
+        <v>5.08923982024805E-6</v>
+      </c>
+      <c r="M8" t="n">
+        <v>5.102249071390669E-6</v>
+      </c>
+      <c r="N8" t="n">
+        <v>5.115325002174015E-6</v>
+      </c>
+      <c r="O8" t="n">
+        <v>5.128468126570593E-6</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
-        <v>2.5000626265687959E-6</v>
-      </c>
-      <c r="C9">
+      <c r="B9" t="n">
+        <v>2.500062626568796E-6</v>
+      </c>
+      <c r="C9" t="n">
         <v>2.5003131642238195E-6</v>
       </c>
-      <c r="D9">
-        <v>2.5006264069149321E-6</v>
-      </c>
-      <c r="E9">
-        <v>2.5031351768089528E-6</v>
-      </c>
-      <c r="F9">
+      <c r="D9" t="n">
+        <v>2.500626406914932E-6</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2.503135176808953E-6</v>
+      </c>
+      <c r="F9" t="n">
         <v>2.5062782269585313E-6</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="n">
         <v>2.5125880662117205E-6</v>
       </c>
-      <c r="H9">
+      <c r="H9" t="n">
         <v>2.5189297571247933E-6</v>
       </c>
-      <c r="I9">
+      <c r="I9" t="n">
         <v>2.5253035414856855E-6</v>
       </c>
-      <c r="J9">
+      <c r="J9" t="n">
         <v>2.5317096635357863E-6</v>
       </c>
-      <c r="K9">
+      <c r="K9" t="n">
         <v>2.5381483700011166E-6</v>
       </c>
-      <c r="L9">
+      <c r="L9" t="n">
         <v>2.5446199101240253E-6</v>
       </c>
-      <c r="M9">
+      <c r="M9" t="n">
         <v>2.551124535695335E-6</v>
       </c>
-      <c r="N9">
+      <c r="N9" t="n">
         <v>2.5576625010870076E-6</v>
       </c>
-      <c r="O9">
+      <c r="O9" t="n">
         <v>2.5642340632852963E-6</v>
       </c>
     </row>
@@ -9929,46 +9930,46 @@
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>3.9992049596537034E-5</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>4.012060261169196E-5</v>
       </c>
-      <c r="D10">
-        <v>4.0282460776091793E-5</v>
-      </c>
-      <c r="E10">
-        <v>4.1625908831475621E-5</v>
-      </c>
-      <c r="F10">
-        <v>4.3436714596330218E-5</v>
-      </c>
-      <c r="G10">
-        <v>4.7576007191208539E-5</v>
-      </c>
-      <c r="H10">
+      <c r="D10" t="n">
+        <v>4.028246077609179E-5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4.162590883147562E-5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4.343671459633022E-5</v>
+      </c>
+      <c r="G10" t="n">
+        <v>4.757600719120854E-5</v>
+      </c>
+      <c r="H10" t="n">
         <v>5.258730320547605E-5</v>
       </c>
-      <c r="I10">
+      <c r="I10" t="n">
         <v>5.877859479488761E-5</v>
       </c>
-      <c r="J10">
-        <v>6.6622264409264367E-5</v>
-      </c>
-      <c r="K10">
-        <v>7.6881341558249442E-5</v>
-      </c>
-      <c r="L10">
-        <v>9.0867832418696116E-5</v>
-      </c>
-      <c r="M10">
+      <c r="J10" t="n">
+        <v>6.662226440926437E-5</v>
+      </c>
+      <c r="K10" t="n">
+        <v>7.688134155824944E-5</v>
+      </c>
+      <c r="L10" t="n">
+        <v>9.086783241869612E-5</v>
+      </c>
+      <c r="M10" t="n">
         <v>1.109766502068123E-4</v>
       </c>
-      <c r="N10">
+      <c r="N10" t="n">
         <v>1.4156436200906655E-4</v>
       </c>
-      <c r="O10">
+      <c r="O10" t="n">
         <v>1.8856251524999575E-4</v>
       </c>
     </row>
@@ -9976,46 +9977,46 @@
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
-        <v>4.0072073687779693E-5</v>
-      </c>
-      <c r="C11">
-        <v>4.0200883937517957E-5</v>
-      </c>
-      <c r="D11">
-        <v>4.0363065980104741E-5</v>
-      </c>
-      <c r="E11">
-        <v>4.1709202275047403E-5</v>
-      </c>
-      <c r="F11">
-        <v>4.3523631462237483E-5</v>
-      </c>
-      <c r="G11">
-        <v>4.7671206781598149E-5</v>
-      </c>
-      <c r="H11">
+      <c r="B11" t="n">
+        <v>4.007207368777969E-5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4.020088393751796E-5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4.036306598010474E-5</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4.17092022750474E-5</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4.352363146223748E-5</v>
+      </c>
+      <c r="G11" t="n">
+        <v>4.767120678159815E-5</v>
+      </c>
+      <c r="H11" t="n">
         <v>5.2692530399190215E-5</v>
       </c>
-      <c r="I11">
-        <v>5.8896210763072183E-5</v>
-      </c>
-      <c r="J11">
-        <v>6.6755575560347301E-5</v>
-      </c>
-      <c r="K11">
+      <c r="I11" t="n">
+        <v>5.889621076307218E-5</v>
+      </c>
+      <c r="J11" t="n">
+        <v>6.67555755603473E-5</v>
+      </c>
+      <c r="K11" t="n">
         <v>7.70351811227075E-5</v>
       </c>
-      <c r="L11">
-        <v>9.1049658951365914E-5</v>
-      </c>
-      <c r="M11">
+      <c r="L11" t="n">
+        <v>9.104965895136591E-5</v>
+      </c>
+      <c r="M11" t="n">
         <v>1.1119871448387613E-4</v>
       </c>
-      <c r="N11">
+      <c r="N11" t="n">
         <v>1.4184763229744667E-4</v>
       </c>
-      <c r="O11">
+      <c r="O11" t="n">
         <v>1.8893982884301096E-4</v>
       </c>
     </row>
@@ -10029,470 +10030,470 @@
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>0.01</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>0.05</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="n">
         <v>0.1</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>0.5</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="H14">
-        <v>3</v>
-      </c>
-      <c r="I14">
-        <v>4</v>
-      </c>
-      <c r="J14">
-        <v>5</v>
-      </c>
-      <c r="K14">
-        <v>6</v>
-      </c>
-      <c r="L14">
-        <v>7</v>
-      </c>
-      <c r="M14">
-        <v>8</v>
-      </c>
-      <c r="N14">
-        <v>9</v>
-      </c>
-      <c r="O14">
-        <v>10</v>
+      <c r="F14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>10.0</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B15">
-        <v>5.3052999575544986E-8</v>
-      </c>
-      <c r="C15">
-        <v>1.951949995624916E-7</v>
-      </c>
-      <c r="D15">
-        <v>5.2051999908093786E-7</v>
-      </c>
-      <c r="E15">
-        <v>2.2022000005786563E-6</v>
-      </c>
-      <c r="F15">
-        <v>5.5055000012923301E-6</v>
-      </c>
-      <c r="G15">
-        <v>9.2092000009658681E-6</v>
-      </c>
-      <c r="H15">
-        <v>1.9924521809025874E-5</v>
-      </c>
-      <c r="I15">
-        <v>1.4910262996592826E-5</v>
-      </c>
-      <c r="J15">
-        <v>2.7598399087612867E-5</v>
-      </c>
-      <c r="K15">
-        <v>2.5825799999328007E-5</v>
-      </c>
-      <c r="L15">
-        <v>3.3947868473823244E-5</v>
-      </c>
-      <c r="M15">
-        <v>4.201578096264256E-5</v>
-      </c>
-      <c r="N15">
-        <v>4.9352899286835812E-5</v>
-      </c>
-      <c r="O15">
-        <v>5.8120863624438767E-5</v>
+      <c r="B15" t="n">
+        <v>5.6556498872497345E-8</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2.674773161782801E-7</v>
+      </c>
+      <c r="D15" t="n">
+        <v>5.555549988624898E-7</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.2601878947253045E-6</v>
+      </c>
+      <c r="F15" t="n">
+        <v>4.554550001113616E-6</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.0833514174588E-5</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1.4586608453340892E-5</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1.9379661479295155E-5</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2.762040196541318E-5</v>
+      </c>
+      <c r="K15" t="n">
+        <v>3.304836478613944E-5</v>
+      </c>
+      <c r="L15" t="n">
+        <v>3.257386707759487E-5</v>
+      </c>
+      <c r="M15" t="n">
+        <v>4.192500316105975E-5</v>
+      </c>
+      <c r="N15" t="n">
+        <v>4.3701329761626446E-5</v>
+      </c>
+      <c r="O15" t="n">
+        <v>5.1993187740245545E-5</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B16">
-        <v>2.5198172541210623E-5</v>
-      </c>
-      <c r="C16">
-        <v>1.2471709358917736E-4</v>
-      </c>
-      <c r="D16">
-        <v>2.4926401445881914E-4</v>
-      </c>
-      <c r="E16">
-        <v>1.249247999088479E-3</v>
-      </c>
-      <c r="F16">
-        <v>2.4924399506511875E-3</v>
-      </c>
-      <c r="G16">
-        <v>5.0008959010232603E-3</v>
-      </c>
-      <c r="H16">
-        <v>7.5321246011189552E-3</v>
-      </c>
-      <c r="I16">
-        <v>1.0043033000941691E-2</v>
-      </c>
-      <c r="J16">
-        <v>1.24341828151737E-2</v>
-      </c>
-      <c r="K16">
-        <v>1.4927312399715908E-2</v>
-      </c>
-      <c r="L16">
-        <v>1.7530462949440797E-2</v>
-      </c>
-      <c r="M16">
-        <v>1.9844224399383107E-2</v>
-      </c>
-      <c r="N16">
-        <v>2.265277277700262E-2</v>
-      </c>
-      <c r="O16">
-        <v>2.4780897255975095E-2</v>
+      <c r="B16" t="n">
+        <v>2.4999725842610157E-5</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1.2475838277891475E-4</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.5124349470765777E-4</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.001247098481548154</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0024882357481775343</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.005037182151318863</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.007550893351761163</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.010044514646708523</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.012503365877211145</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.015014466201357263</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.017625879008384415</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.02002428957703305</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.022559430785684714</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.02510142238492802</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B17">
-        <v>4.0320435868606631E-4</v>
-      </c>
-      <c r="C17">
-        <v>1.9972173649536423E-3</v>
-      </c>
-      <c r="D17">
-        <v>3.9945042915228938E-3</v>
-      </c>
-      <c r="E17">
-        <v>2.0172772350438392E-2</v>
-      </c>
-      <c r="F17">
-        <v>4.0652412442878622E-2</v>
-      </c>
-      <c r="G17">
-        <v>8.3445187334836066E-2</v>
-      </c>
-      <c r="H17">
-        <v>0.12976538929197567</v>
-      </c>
-      <c r="I17">
-        <v>0.18046430452231271</v>
-      </c>
-      <c r="J17">
-        <v>0.23545454486439571</v>
-      </c>
-      <c r="K17">
-        <v>0.30097816728044913</v>
-      </c>
-      <c r="L17">
-        <v>0.3862457795207892</v>
-      </c>
-      <c r="M17">
-        <v>0.4921480222665538</v>
-      </c>
-      <c r="N17">
-        <v>0.67957641154432258</v>
-      </c>
-      <c r="O17">
-        <v>0.92836274226733606</v>
+      <c r="B17" t="n">
+        <v>4.0005947481685605E-4</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0019977536037045413</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.004027532218113502</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.020141960634662767</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.04058818719195815</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.08430244594592441</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.13036088034427626</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.1801725543096167</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.23665874565699635</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.3026989387776815</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.39344057923141396</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.5006499851577411</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.6680580249704112</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.9886959964498585</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B18">
-        <v>4.0364547061467115E-4</v>
-      </c>
-      <c r="C18">
-        <v>1.9991660364392211E-3</v>
-      </c>
-      <c r="D18">
-        <v>4.0003321339381779E-3</v>
-      </c>
-      <c r="E18">
-        <v>2.0203058320588871E-2</v>
-      </c>
-      <c r="F18">
-        <v>4.0761953107885399E-2</v>
-      </c>
-      <c r="G18">
-        <v>8.3654013745533162E-2</v>
-      </c>
-      <c r="H18">
-        <v>0.12954368260921842</v>
-      </c>
-      <c r="I18">
-        <v>0.17967225697411912</v>
-      </c>
-      <c r="J18">
-        <v>0.23186089701706714</v>
-      </c>
-      <c r="K18">
-        <v>0.29273446363355549</v>
-      </c>
-      <c r="L18">
-        <v>0.37046694461883078</v>
-      </c>
-      <c r="M18">
-        <v>0.45924528388905989</v>
-      </c>
-      <c r="N18">
-        <v>0.60825547025492377</v>
-      </c>
-      <c r="O18">
-        <v>0.79821328379292256</v>
+      <c r="B18" t="n">
+        <v>4.0054584081852E-4</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.002000169942803087</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.004031929056932646</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.020185723410108665</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.040658152415147725</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.08447548133942741</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.13058307707402503</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.1797027512355409</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.23377438689469135</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.29593229655823156</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.37588663794289573</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.467165685288567</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.6013951825876653</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.8440608167711069</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B19">
-        <v>8.321010548415237E-4</v>
-      </c>
-      <c r="C19">
-        <v>4.1212956899816036E-3</v>
-      </c>
-      <c r="D19">
-        <v>8.2446209599189718E-3</v>
-      </c>
-      <c r="E19">
-        <v>4.1627280870116322E-2</v>
-      </c>
-      <c r="F19">
-        <v>8.3912311001416495E-2</v>
-      </c>
-      <c r="G19">
-        <v>0.17210930618139347</v>
-      </c>
-      <c r="H19">
-        <v>0.26686112102412207</v>
-      </c>
-      <c r="I19">
-        <v>0.37019450476037014</v>
-      </c>
-      <c r="J19">
-        <v>0.47977722309572413</v>
-      </c>
-      <c r="K19">
-        <v>0.60866576911371983</v>
-      </c>
-      <c r="L19">
-        <v>0.77427713495753459</v>
-      </c>
-      <c r="M19">
-        <v>0.97127954633595937</v>
-      </c>
-      <c r="N19">
-        <v>1.3105340074755358</v>
-      </c>
-      <c r="O19">
-        <v>1.7514150441798582</v>
+      <c r="B19" t="n">
+        <v>8.256615979768587E-4</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.004122949406602721</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.008311260324752668</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.04157704271421431</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.08373912990528451</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.17382594295084527</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.2685094373785158</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.36993919985334545</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.48296411883086426</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.6136787499020564</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.7869856700497717</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.9878818850265021</v>
+      </c>
+      <c r="N19" t="n">
+        <v>1.2920563396735227</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1.8579102287936338</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B20">
-        <v>4.9074073681452791E-6</v>
-      </c>
-      <c r="C20">
-        <v>4.8749999890732173E-6</v>
-      </c>
-      <c r="D20">
-        <v>4.9056603686967546E-6</v>
-      </c>
-      <c r="E20">
-        <v>4.888888890173508E-6</v>
-      </c>
-      <c r="F20">
-        <v>4.910714286866999E-6</v>
-      </c>
-      <c r="G20">
-        <v>4.893617021789842E-6</v>
-      </c>
-      <c r="H20">
-        <v>4.9264705881258604E-6</v>
-      </c>
-      <c r="I20">
-        <v>4.8717948716323713E-6</v>
-      </c>
-      <c r="J20">
-        <v>5.0019392384719978E-6</v>
-      </c>
-      <c r="K20">
-        <v>4.8863636362364917E-6</v>
-      </c>
-      <c r="L20">
-        <v>4.9019607841775075E-6</v>
-      </c>
-      <c r="M20">
-        <v>4.9090909089649295E-6</v>
-      </c>
-      <c r="N20">
-        <v>4.9226661930363504E-6</v>
-      </c>
-      <c r="O20">
-        <v>4.9284262989838699E-6</v>
+      <c r="B20" t="n">
+        <v>4.956140252072257E-6</v>
+      </c>
+      <c r="C20" t="n">
+        <v>4.953703745903768E-6</v>
+      </c>
+      <c r="D20" t="n">
+        <v>4.955357132710948E-6</v>
+      </c>
+      <c r="E20" t="n">
+        <v>4.951371632701932E-6</v>
+      </c>
+      <c r="F20" t="n">
+        <v>4.945652175122286E-6</v>
+      </c>
+      <c r="G20" t="n">
+        <v>4.954545455655541E-6</v>
+      </c>
+      <c r="H20" t="n">
+        <v>4.949494950271118E-6</v>
+      </c>
+      <c r="I20" t="n">
+        <v>4.969738504792037E-6</v>
+      </c>
+      <c r="J20" t="n">
+        <v>4.955752212642865E-6</v>
+      </c>
+      <c r="K20" t="n">
+        <v>4.987718640400393E-6</v>
+      </c>
+      <c r="L20" t="n">
+        <v>4.965524137212284E-6</v>
+      </c>
+      <c r="M20" t="n">
+        <v>4.963575216253181E-6</v>
+      </c>
+      <c r="N20" t="n">
+        <v>4.999321147453834E-6</v>
+      </c>
+      <c r="O20" t="n">
+        <v>5.0088924051931175E-6</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B21">
-        <v>2.4999502990912026E-6</v>
-      </c>
-      <c r="C21">
-        <v>2.4999498593059366E-6</v>
-      </c>
-      <c r="D21">
-        <v>2.4999497978009777E-6</v>
-      </c>
-      <c r="E21">
-        <v>2.4999499190508799E-6</v>
-      </c>
-      <c r="F21">
-        <v>2.4999497998499369E-6</v>
-      </c>
-      <c r="G21">
-        <v>2.4999499604795028E-6</v>
-      </c>
-      <c r="H21">
-        <v>2.499984922525705E-6</v>
-      </c>
-      <c r="I21">
-        <v>2.4999739286992698E-6</v>
-      </c>
-      <c r="J21">
-        <v>2.5000645673528857E-6</v>
-      </c>
-      <c r="K21">
-        <v>2.4999497072488871E-6</v>
-      </c>
-      <c r="L21">
-        <v>2.4999948544765424E-6</v>
-      </c>
-      <c r="M21">
-        <v>2.4999966968822205E-6</v>
-      </c>
-      <c r="N21">
-        <v>2.5002268569154158E-6</v>
-      </c>
-      <c r="O21">
-        <v>2.5000568324207265E-6</v>
+      <c r="B21" t="n">
+        <v>2.4999750842361E-6</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2.5000192388520244E-6</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2.4999751210726543E-6</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2.4999908255903056E-6</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2.4999748551049022E-6</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2.499986433765669E-6</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2.5000321598524756E-6</v>
+      </c>
+      <c r="I21" t="n">
+        <v>2.50001502382784E-6</v>
+      </c>
+      <c r="J21" t="n">
+        <v>2.5000936296861383E-6</v>
+      </c>
+      <c r="K21" t="n">
+        <v>2.500077559388507E-6</v>
+      </c>
+      <c r="L21" t="n">
+        <v>2.500023614715353E-6</v>
+      </c>
+      <c r="M21" t="n">
+        <v>2.5001103648553105E-6</v>
+      </c>
+      <c r="N21" t="n">
+        <v>2.5000258095153837E-6</v>
+      </c>
+      <c r="O21" t="n">
+        <v>2.5000689124902164E-6</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B22">
-        <v>4.0010683786207105E-5</v>
-      </c>
-      <c r="C22">
-        <v>4.0075190945387755E-5</v>
-      </c>
-      <c r="D22">
-        <v>4.0153136238200314E-5</v>
-      </c>
-      <c r="E22">
-        <v>4.084621967378051E-5</v>
-      </c>
-      <c r="F22">
-        <v>4.1800926969075995E-5</v>
-      </c>
-      <c r="G22">
-        <v>4.3965918781160856E-5</v>
-      </c>
-      <c r="H22">
-        <v>4.6952591336793666E-5</v>
-      </c>
-      <c r="I22">
-        <v>5.0858364748056567E-5</v>
-      </c>
-      <c r="J22">
-        <v>5.5810805807873074E-5</v>
-      </c>
-      <c r="K22">
-        <v>6.1857507055875668E-5</v>
-      </c>
-      <c r="L22">
-        <v>7.0854497158130117E-5</v>
-      </c>
-      <c r="M22">
-        <v>8.3303549236259756E-5</v>
-      </c>
-      <c r="N22">
-        <v>1.0658845029386916E-4</v>
-      </c>
-      <c r="O22">
-        <v>1.3885628893791336E-4</v>
+      <c r="B22" t="n">
+        <v>4.001697752754841E-5</v>
+      </c>
+      <c r="C22" t="n">
+        <v>4.007766163125593E-5</v>
+      </c>
+      <c r="D22" t="n">
+        <v>4.016579442817706E-5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>4.086019189546383E-5</v>
+      </c>
+      <c r="F22" t="n">
+        <v>4.181745487140516E-5</v>
+      </c>
+      <c r="G22" t="n">
+        <v>4.4191956210853605E-5</v>
+      </c>
+      <c r="H22" t="n">
+        <v>4.714525479574751E-5</v>
+      </c>
+      <c r="I22" t="n">
+        <v>5.0784971637748504E-5</v>
+      </c>
+      <c r="J22" t="n">
+        <v>5.56931222568449E-5</v>
+      </c>
+      <c r="K22" t="n">
+        <v>6.195764167823808E-5</v>
+      </c>
+      <c r="L22" t="n">
+        <v>7.213612246736447E-5</v>
+      </c>
+      <c r="M22" t="n">
+        <v>8.452216335897243E-5</v>
+      </c>
+      <c r="N22" t="n">
+        <v>1.0502163854202326E-4</v>
+      </c>
+      <c r="O22" t="n">
+        <v>1.4753427753553324E-4</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B23">
-        <v>4.0023036329150347E-5</v>
-      </c>
-      <c r="C23">
-        <v>4.0155655794220751E-5</v>
-      </c>
-      <c r="D23">
-        <v>4.0303532622898799E-5</v>
-      </c>
-      <c r="E23">
-        <v>4.159204957861391E-5</v>
-      </c>
-      <c r="F23">
-        <v>4.3331370972883667E-5</v>
-      </c>
-      <c r="G23">
-        <v>4.6877690068627158E-5</v>
-      </c>
-      <c r="H23">
-        <v>5.1152466519599069E-5</v>
-      </c>
-      <c r="I23">
-        <v>5.6384865605173159E-5</v>
-      </c>
-      <c r="J23">
-        <v>6.2440004525966507E-5</v>
-      </c>
-      <c r="K23">
-        <v>6.942397223286117E-5</v>
-      </c>
-      <c r="L23">
-        <v>7.9733208944972276E-5</v>
-      </c>
-      <c r="M23">
-        <v>9.2902859689569897E-5</v>
-      </c>
-      <c r="N23">
-        <v>1.1713178736239443E-4</v>
-      </c>
-      <c r="O23">
-        <v>1.5044283145923109E-4</v>
+      <c r="B23" t="n">
+        <v>4.003638573237961E-5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>4.015281298314365E-5</v>
+      </c>
+      <c r="D23" t="n">
+        <v>4.0327442727025513E-5</v>
+      </c>
+      <c r="E23" t="n">
+        <v>4.1659702630960286E-5</v>
+      </c>
+      <c r="F23" t="n">
+        <v>4.32629342842269E-5</v>
+      </c>
+      <c r="G23" t="n">
+        <v>4.713154858279659E-5</v>
+      </c>
+      <c r="H23" t="n">
+        <v>5.151701006969011E-5</v>
+      </c>
+      <c r="I23" t="n">
+        <v>5.635003786277244E-5</v>
+      </c>
+      <c r="J23" t="n">
+        <v>6.247717934185371E-5</v>
+      </c>
+      <c r="K23" t="n">
+        <v>6.974274236602507E-5</v>
+      </c>
+      <c r="L23" t="n">
+        <v>8.099998790072215E-5</v>
+      </c>
+      <c r="M23" t="n">
+        <v>9.431726597934289E-5</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1.1564607043085904E-4</v>
+      </c>
+      <c r="O23" t="n">
+        <v>1.590883599449693E-4</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
File structure for faults
</commit_message>
<xml_diff>
--- a/CharacteristicsDependancy.xlsx
+++ b/CharacteristicsDependancy.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
   <si>
     <t>МО числа требований 1 класса в S1</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>L01</t>
+  </si>
+  <si>
+    <t>Характеристики узла в ненадежной среде</t>
   </si>
 </sst>
 </file>
@@ -318,46 +321,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>5.055049888499384E-8</c:v>
+                  <c:v>4.9048999060908056E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5275250198559155E-7</c:v>
+                  <c:v>2.8528500258625804E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.2552499894030867E-7</c:v>
+                  <c:v>4.9549499887187602E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4274249975574694E-6</c:v>
+                  <c:v>2.8027999972643141E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0050000011299025E-6</c:v>
+                  <c:v>5.2052000013562587E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0104561073004199E-5</c:v>
+                  <c:v>1.0910900002146794E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4154237666283881E-5</c:v>
+                  <c:v>1.7676024037645201E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3540520268883593E-5</c:v>
+                  <c:v>1.8059970228732063E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.1986968534882536E-5</c:v>
+                  <c:v>2.2635693099275753E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.6397066036996172E-5</c:v>
+                  <c:v>2.7692241029066868E-5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.7234801652510124E-5</c:v>
+                  <c:v>3.4441718454659587E-5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.8169881637098382E-5</c:v>
+                  <c:v>4.3612232669080537E-5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.8657900478001957E-5</c:v>
+                  <c:v>3.7657780902416348E-5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.0605781433388735E-5</c:v>
+                  <c:v>4.3167063878133498E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -379,11 +382,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85944960"/>
-        <c:axId val="85950848"/>
+        <c:axId val="118254208"/>
+        <c:axId val="118264192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85944960"/>
+        <c:axId val="118254208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,7 +428,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85950848"/>
+        <c:crossAx val="118264192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -433,7 +436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85950848"/>
+        <c:axId val="118264192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,7 +487,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85944960"/>
+        <c:crossAx val="118254208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -727,46 +730,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>2.5146372331511488E-5</c:v>
+                  <c:v>2.5081807840961791E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2519882278914414E-4</c:v>
+                  <c:v>1.2468831280532789E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4950926217452772E-4</c:v>
+                  <c:v>2.4729454966766437E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2540527979586916E-3</c:v>
+                  <c:v>1.2457695229734199E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.500948448176893E-3</c:v>
+                  <c:v>2.4991113985155201E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.999044051306259E-3</c:v>
+                  <c:v>4.9968418513071326E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.4759685017475831E-3</c:v>
+                  <c:v>7.4919840884407419E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.981051026116081E-3</c:v>
+                  <c:v>9.992935393649597E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.241307930974276E-2</c:v>
+                  <c:v>1.2500285083555331E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4917920180985145E-2</c:v>
+                  <c:v>1.4965159970619887E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.7592828770171234E-2</c:v>
+                  <c:v>1.7473769255855049E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.00191561446912E-2</c:v>
+                  <c:v>2.006120870660311E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.2528095645113891E-2</c:v>
+                  <c:v>2.2500221412120811E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.5004698670798513E-2</c:v>
+                  <c:v>2.4953550056333713E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -788,11 +791,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98981760"/>
-        <c:axId val="98983296"/>
+        <c:axId val="118122368"/>
+        <c:axId val="118123904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98981760"/>
+        <c:axId val="118122368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -834,7 +837,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98983296"/>
+        <c:crossAx val="118123904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -842,7 +845,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98983296"/>
+        <c:axId val="118123904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -893,7 +896,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98981760"/>
+        <c:crossAx val="118122368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1136,46 +1139,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>4.0240060746434063E-4</c:v>
+                  <c:v>4.0137577229212699E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0049662717940087E-3</c:v>
+                  <c:v>1.996862863588687E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9989030279538535E-3</c:v>
+                  <c:v>3.9630990359579002E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0251985162569892E-2</c:v>
+                  <c:v>2.0113739292667552E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.078256456054262E-2</c:v>
+                  <c:v>4.0781348728509144E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.3530980395682478E-2</c:v>
+                  <c:v>8.3618474460216669E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12856699073613845</c:v>
+                  <c:v>0.12907653955521894</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.17878199817288648</c:v>
+                  <c:v>0.17907405190049056</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.23337487984798636</c:v>
+                  <c:v>0.23681388735035672</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.30012422445385051</c:v>
+                  <c:v>0.30268608175681105</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.39010079627631128</c:v>
+                  <c:v>0.3851286413763314</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.49882483882835771</c:v>
+                  <c:v>0.50360173957207677</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.6717939473618797</c:v>
+                  <c:v>0.66945571617692134</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.96912283624427087</c:v>
+                  <c:v>0.95761049868487069</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1197,11 +1200,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99005568"/>
-        <c:axId val="99007104"/>
+        <c:axId val="118150272"/>
+        <c:axId val="118151808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99005568"/>
+        <c:axId val="118150272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1243,7 +1246,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99007104"/>
+        <c:crossAx val="118151808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1251,7 +1254,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99007104"/>
+        <c:axId val="118151808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1302,7 +1305,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99005568"/>
+        <c:crossAx val="118150272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1545,46 +1548,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>4.0280395689913033E-4</c:v>
+                  <c:v>4.0176918347660078E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0070128856621789E-3</c:v>
+                  <c:v>1.999266148260904E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0023433828666778E-3</c:v>
+                  <c:v>3.9670907800541458E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.029219346947702E-2</c:v>
+                  <c:v>2.0162045570326539E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0843918710783203E-2</c:v>
+                  <c:v>4.0910670419273418E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.3834791966542574E-2</c:v>
+                  <c:v>8.3862521440954949E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12866537912900561</c:v>
+                  <c:v>0.12905189121937882</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.17846913756618224</c:v>
+                  <c:v>0.1783473928176858</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.22992966445804944</c:v>
+                  <c:v>0.23279844723496898</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.29323436026936339</c:v>
+                  <c:v>0.29503997047216329</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.37235032954549385</c:v>
+                  <c:v>0.36814032853103029</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.46422241711268031</c:v>
+                  <c:v>0.46820242973148973</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.60312896908065161</c:v>
+                  <c:v>0.60171046195262834</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.82977921639565511</c:v>
+                  <c:v>0.82121099129335562</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1606,11 +1609,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99366784"/>
-        <c:axId val="99368320"/>
+        <c:axId val="118313344"/>
+        <c:axId val="118314880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99366784"/>
+        <c:axId val="118313344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1652,7 +1655,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99368320"/>
+        <c:crossAx val="118314880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1660,7 +1663,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99368320"/>
+        <c:axId val="118314880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1711,7 +1714,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99366784"/>
+        <c:crossAx val="118313344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1832,7 +1835,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1949,46 +1951,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>8.3040148719386742E-4</c:v>
+                  <c:v>8.2827581260875053E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1374307327473169E-3</c:v>
+                  <c:v>4.1211026096575048E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.2512811979939989E-3</c:v>
+                  <c:v>8.1779798606785824E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1800658855003156E-2</c:v>
+                  <c:v>4.1524357185964776E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.413243671950385E-2</c:v>
+                  <c:v>8.4196335746299436E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17237492097460433</c:v>
+                  <c:v>0.1724887486524809</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.26472249260455794</c:v>
+                  <c:v>0.26563809088707613</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.36725572728545364</c:v>
+                  <c:v>0.36743244008205467</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.47573961058431347</c:v>
+                  <c:v>0.48213525536198032</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.60830290197023607</c:v>
+                  <c:v>0.61271890444062327</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.7800811893936288</c:v>
+                  <c:v>0.77077718088167146</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.98311458196736634</c:v>
+                  <c:v>0.99190899024283874</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.2974996699881234</c:v>
+                  <c:v>1.2937040573225729</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.8239573570921577</c:v>
+                  <c:v>1.8038182070984381</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2010,11 +2012,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99415552"/>
-        <c:axId val="99417088"/>
+        <c:axId val="118357376"/>
+        <c:axId val="118686848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99415552"/>
+        <c:axId val="118357376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2056,7 +2058,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99417088"/>
+        <c:crossAx val="118686848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2064,7 +2066,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99417088"/>
+        <c:axId val="118686848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2115,7 +2117,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99415552"/>
+        <c:crossAx val="118357376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2129,7 +2131,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2241,7 +2242,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2358,46 +2358,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>4.9509802829517389E-6</c:v>
+                  <c:v>4.9494948547319406E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9509804310511366E-6</c:v>
+                  <c:v>4.956521784063902E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9528301786921439E-6</c:v>
+                  <c:v>4.949999988730031E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9489795868569583E-6</c:v>
+                  <c:v>4.955752207552296E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.950495050622548E-6</c:v>
+                  <c:v>4.9664624364194316E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9509803931751156E-6</c:v>
+                  <c:v>4.9545454555202951E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9484536090434967E-6</c:v>
+                  <c:v>4.9648703378943084E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9747781785362418E-6</c:v>
+                  <c:v>4.9603331061359007E-6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0116584585591007E-6</c:v>
+                  <c:v>4.9564051754926186E-6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.9582726873752629E-6</c:v>
+                  <c:v>4.9751345058976492E-6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.9541685898022243E-6</c:v>
+                  <c:v>4.9841500425583179E-6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.9956286406588135E-6</c:v>
+                  <c:v>5.0185328764493592E-6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.9965018616688513E-6</c:v>
+                  <c:v>4.9455387614358618E-6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.9969855289089898E-6</c:v>
+                  <c:v>4.9857148871649392E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2419,11 +2419,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99787520"/>
-        <c:axId val="99789056"/>
+        <c:axId val="118733440"/>
+        <c:axId val="119013760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99787520"/>
+        <c:axId val="118733440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2465,7 +2465,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99789056"/>
+        <c:crossAx val="119013760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2473,7 +2473,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99789056"/>
+        <c:axId val="119013760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2524,7 +2524,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99787520"/>
+        <c:crossAx val="118733440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2538,7 +2538,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2650,7 +2649,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2767,46 +2765,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>2.4999752284329216E-6</c:v>
+                  <c:v>2.4999751656096022E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4999749958045981E-6</c:v>
+                  <c:v>2.4999748937557025E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4999749478196213E-6</c:v>
+                  <c:v>2.4999747233910028E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4999750520543396E-6</c:v>
+                  <c:v>2.4999748862035987E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4999749829182945E-6</c:v>
+                  <c:v>2.4999749646274405E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5000222602217147E-6</c:v>
+                  <c:v>2.4999749600882562E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5000385278692137E-6</c:v>
+                  <c:v>2.5000111453204574E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.500004263605632E-6</c:v>
+                  <c:v>2.4999854580125439E-6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.5001189443756275E-6</c:v>
+                  <c:v>2.500047662200179E-6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.5000705714470675E-6</c:v>
+                  <c:v>2.5000358811654419E-6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.4999889912953436E-6</c:v>
+                  <c:v>2.5000404307331774E-6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.5000902220240315E-6</c:v>
+                  <c:v>2.500070935687037E-6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.5002259692450114E-6</c:v>
+                  <c:v>2.5000550714419007E-6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.5000805855673704E-6</c:v>
+                  <c:v>2.500087642112427E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2828,11 +2826,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100927360"/>
-        <c:axId val="100928896"/>
+        <c:axId val="119027584"/>
+        <c:axId val="119029120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100927360"/>
+        <c:axId val="119027584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2874,7 +2872,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100928896"/>
+        <c:crossAx val="119029120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2882,7 +2880,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100928896"/>
+        <c:axId val="119029120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2933,7 +2931,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100927360"/>
+        <c:crossAx val="119027584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2947,7 +2945,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3059,7 +3056,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3176,46 +3172,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>4.0017457678376392E-5</c:v>
+                  <c:v>4.0016344215596806E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.008369221654161E-5</c:v>
+                  <c:v>4.0080429027723161E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0156904357959443E-5</c:v>
+                  <c:v>4.015254670999158E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0852832443472262E-5</c:v>
+                  <c:v>4.0849487731617519E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1809458265669958E-5</c:v>
+                  <c:v>4.1821072855603256E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.4065252957344062E-5</c:v>
+                  <c:v>4.4138915066023128E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6820867588231518E-5</c:v>
+                  <c:v>4.699489373597177E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.0627461723318868E-5</c:v>
+                  <c:v>5.0658782731821844E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.5173630658832748E-5</c:v>
+                  <c:v>5.5814282923136672E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.1591872283150496E-5</c:v>
+                  <c:v>6.2118249407865322E-5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.143695697524598E-5</c:v>
+                  <c:v>7.0643066452809666E-5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.4112218347656806E-5</c:v>
+                  <c:v>8.4810669962435379E-5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.0577396554133889E-4</c:v>
+                  <c:v>1.0550178571475082E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.4484804514320858E-4</c:v>
+                  <c:v>1.4325541148922787E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3237,11 +3233,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100963456"/>
-        <c:axId val="100964992"/>
+        <c:axId val="119059584"/>
+        <c:axId val="119061120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100963456"/>
+        <c:axId val="119059584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3283,7 +3279,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100964992"/>
+        <c:crossAx val="119061120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3291,7 +3287,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100964992"/>
+        <c:axId val="119061120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3342,7 +3338,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100963456"/>
+        <c:crossAx val="119059584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3356,7 +3352,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3468,7 +3463,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3585,46 +3579,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>4.0028705396666646E-5</c:v>
+                  <c:v>4.0031776244610565E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.015743726158511E-5</c:v>
+                  <c:v>4.0162969713749125E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0288397802108844E-5</c:v>
+                  <c:v>4.0285259883256785E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1656300029478152E-5</c:v>
+                  <c:v>4.1625105368083706E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3255284577197783E-5</c:v>
+                  <c:v>4.3368153433019168E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.7083107891783774E-5</c:v>
+                  <c:v>4.7106686392645086E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.109096694878073E-5</c:v>
+                  <c:v>5.1152927869688534E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6224655892972187E-5</c:v>
+                  <c:v>5.6164910272107087E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.1644229753759889E-5</c:v>
+                  <c:v>6.2359333998067068E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9514568180009551E-5</c:v>
+                  <c:v>6.9919472106117701E-5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.0130625358370631E-5</c:v>
+                  <c:v>7.943978860866048E-5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.3659800316996328E-5</c:v>
+                  <c:v>9.4428291046037691E-5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1638946830480306E-4</c:v>
+                  <c:v>1.1615122491173048E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.5639712694719152E-4</c:v>
+                  <c:v>1.5472318207825322E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3646,11 +3640,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101396864"/>
-        <c:axId val="101398400"/>
+        <c:axId val="120537472"/>
+        <c:axId val="120539008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101396864"/>
+        <c:axId val="120537472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3692,7 +3686,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101398400"/>
+        <c:crossAx val="120539008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3700,7 +3694,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101398400"/>
+        <c:axId val="120539008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3751,7 +3745,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101396864"/>
+        <c:crossAx val="120537472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3765,7 +3759,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8842,14 +8835,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4572000</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8872,14 +8865,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8902,14 +8895,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8932,14 +8925,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>195262</xdr:rowOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8962,14 +8955,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8992,14 +8985,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9022,14 +9015,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9052,14 +9045,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9082,14 +9075,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9366,7 +9359,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9374,10 +9367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52:B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9920,46 +9913,46 @@
         <v>0</v>
       </c>
       <c r="B15" t="n">
-        <v>4.9048999060908056E-8</v>
+        <v>4.554549915794895E-8</v>
       </c>
       <c r="C15" t="n">
-        <v>2.8528500258625804E-7</v>
+        <v>3.153150024953254E-7</v>
       </c>
       <c r="D15" t="n">
-        <v>4.95494998871876E-7</v>
+        <v>4.4043999906977724E-7</v>
       </c>
       <c r="E15" t="n">
-        <v>2.802799997264314E-6</v>
+        <v>2.7527499986373163E-6</v>
       </c>
       <c r="F15" t="n">
-        <v>5.205200001356259E-6</v>
+        <v>5.41178865227535E-6</v>
       </c>
       <c r="G15" t="n">
-        <v>1.0910900002146794E-5</v>
+        <v>9.421772055399135E-6</v>
       </c>
       <c r="H15" t="n">
-        <v>1.76760240376452E-5</v>
+        <v>1.3599784611960377E-5</v>
       </c>
       <c r="I15" t="n">
-        <v>1.8059970228732063E-5</v>
+        <v>1.87394015698027E-5</v>
       </c>
       <c r="J15" t="n">
-        <v>2.2635693099275753E-5</v>
+        <v>2.2789002662449432E-5</v>
       </c>
       <c r="K15" t="n">
-        <v>2.769224102906687E-5</v>
+        <v>2.98399157221502E-5</v>
       </c>
       <c r="L15" t="n">
-        <v>3.4441718454659587E-5</v>
+        <v>3.292085855291904E-5</v>
       </c>
       <c r="M15" t="n">
-        <v>4.361223266908054E-5</v>
+        <v>3.715538335434872E-5</v>
       </c>
       <c r="N15" t="n">
-        <v>3.765778090241635E-5</v>
+        <v>5.10153773876514E-5</v>
       </c>
       <c r="O15" t="n">
-        <v>4.31670638781335E-5</v>
+        <v>5.122066852764156E-5</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -9967,46 +9960,46 @@
         <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>2.508180784096179E-5</v>
+        <v>2.509306910387978E-5</v>
       </c>
       <c r="C16" t="n">
-        <v>1.246883128053279E-4</v>
+        <v>1.2434421905072382E-4</v>
       </c>
       <c r="D16" t="n">
-        <v>2.4729454966766437E-4</v>
+        <v>2.4906131468886223E-4</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0012457695229734199</v>
+        <v>0.0012516629104529905</v>
       </c>
       <c r="F16" t="n">
-        <v>0.00249911139851552</v>
+        <v>0.002497344848180885</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0049968418513071326</v>
+        <v>0.005020715701306257</v>
       </c>
       <c r="H16" t="n">
-        <v>0.007491984088440742</v>
+        <v>0.007459988149168892</v>
       </c>
       <c r="I16" t="n">
-        <v>0.009992935393649597</v>
+        <v>0.010041131102069828</v>
       </c>
       <c r="J16" t="n">
-        <v>0.012500285083555331</v>
+        <v>0.012470252681477884</v>
       </c>
       <c r="K16" t="n">
-        <v>0.014965159970619887</v>
+        <v>0.01502400900223684</v>
       </c>
       <c r="L16" t="n">
-        <v>0.01747376925585505</v>
+        <v>0.01742826304431555</v>
       </c>
       <c r="M16" t="n">
-        <v>0.02006120870660311</v>
+        <v>0.019948101726693573</v>
       </c>
       <c r="N16" t="n">
-        <v>0.02250022141212081</v>
+        <v>0.02255030072224286</v>
       </c>
       <c r="O16" t="n">
-        <v>0.024953550056333713</v>
+        <v>0.024883464576189448</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -10014,46 +10007,46 @@
         <v>2</v>
       </c>
       <c r="B17" t="n">
-        <v>4.01375772292127E-4</v>
+        <v>4.015465269408129E-4</v>
       </c>
       <c r="C17" t="n">
-        <v>0.001996862863588687</v>
+        <v>0.001991155160460868</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0039630990359579</v>
+        <v>0.0039914707508654996</v>
       </c>
       <c r="E17" t="n">
-        <v>0.020113739292667552</v>
+        <v>0.020210023597246534</v>
       </c>
       <c r="F17" t="n">
-        <v>0.040781348728509144</v>
+        <v>0.04074758298746837</v>
       </c>
       <c r="G17" t="n">
-        <v>0.08361847446021667</v>
+        <v>0.08383250685898734</v>
       </c>
       <c r="H17" t="n">
-        <v>0.12907653955521894</v>
+        <v>0.12850199168579332</v>
       </c>
       <c r="I17" t="n">
-        <v>0.17907405190049056</v>
+        <v>0.18073619981804942</v>
       </c>
       <c r="J17" t="n">
-        <v>0.23681388735035672</v>
+        <v>0.23585618778691608</v>
       </c>
       <c r="K17" t="n">
-        <v>0.30268608175681105</v>
+        <v>0.3036381716269749</v>
       </c>
       <c r="L17" t="n">
-        <v>0.3851286413763314</v>
+        <v>0.3851170402163171</v>
       </c>
       <c r="M17" t="n">
-        <v>0.5036017395720768</v>
+        <v>0.4939457742635197</v>
       </c>
       <c r="N17" t="n">
-        <v>0.6694557161769213</v>
+        <v>0.6715080316388303</v>
       </c>
       <c r="O17" t="n">
-        <v>0.9576104986848707</v>
+        <v>0.9470797943003115</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -10061,46 +10054,46 @@
         <v>3</v>
       </c>
       <c r="B18" t="n">
-        <v>4.017691834766008E-4</v>
+        <v>4.0191777440302256E-4</v>
       </c>
       <c r="C18" t="n">
-        <v>0.001999266148260904</v>
+        <v>0.0019937644191427998</v>
       </c>
       <c r="D18" t="n">
-        <v>0.003967090780054146</v>
+        <v>0.003996680006545663</v>
       </c>
       <c r="E18" t="n">
-        <v>0.02016204557032654</v>
+        <v>0.020253767610277112</v>
       </c>
       <c r="F18" t="n">
-        <v>0.04091067041927342</v>
+        <v>0.040859566531454256</v>
       </c>
       <c r="G18" t="n">
-        <v>0.08386252144095495</v>
+        <v>0.08413090487735086</v>
       </c>
       <c r="H18" t="n">
-        <v>0.12905189121937882</v>
+        <v>0.1285644249315754</v>
       </c>
       <c r="I18" t="n">
-        <v>0.1783473928176858</v>
+        <v>0.18004552503524726</v>
       </c>
       <c r="J18" t="n">
-        <v>0.23279844723496898</v>
+        <v>0.2323477199249933</v>
       </c>
       <c r="K18" t="n">
-        <v>0.2950399704721633</v>
+        <v>0.2958003223891175</v>
       </c>
       <c r="L18" t="n">
-        <v>0.3681403285310303</v>
+        <v>0.36709548724190344</v>
       </c>
       <c r="M18" t="n">
-        <v>0.46820242973148973</v>
+        <v>0.45959885135538725</v>
       </c>
       <c r="N18" t="n">
-        <v>0.6017104619526283</v>
+        <v>0.6021708244852496</v>
       </c>
       <c r="O18" t="n">
-        <v>0.8212109912933556</v>
+        <v>0.811879830764057</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -10108,46 +10101,46 @@
         <v>4</v>
       </c>
       <c r="B19" t="n">
-        <v>8.282758126087505E-4</v>
+        <v>8.286029159468731E-4</v>
       </c>
       <c r="C19" t="n">
-        <v>0.004121102609657505</v>
+        <v>0.004109579113656887</v>
       </c>
       <c r="D19" t="n">
-        <v>0.008177979860678582</v>
+        <v>0.008237652512099094</v>
       </c>
       <c r="E19" t="n">
-        <v>0.041524357185964776</v>
+        <v>0.041718206867975276</v>
       </c>
       <c r="F19" t="n">
-        <v>0.08419633574629944</v>
+        <v>0.08410990615575578</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1724887486524809</v>
+        <v>0.17299354920969987</v>
       </c>
       <c r="H19" t="n">
-        <v>0.26563809088707613</v>
+        <v>0.26454000455114957</v>
       </c>
       <c r="I19" t="n">
-        <v>0.36743244008205467</v>
+        <v>0.3708415953569363</v>
       </c>
       <c r="J19" t="n">
-        <v>0.4821352553619803</v>
+        <v>0.48069694939604973</v>
       </c>
       <c r="K19" t="n">
-        <v>0.6127189044406233</v>
+        <v>0.6144923429340514</v>
       </c>
       <c r="L19" t="n">
-        <v>0.7707771808816715</v>
+        <v>0.769673711361089</v>
       </c>
       <c r="M19" t="n">
-        <v>0.9919089902428387</v>
+        <v>0.9735298827289549</v>
       </c>
       <c r="N19" t="n">
-        <v>1.2937040573225729</v>
+        <v>1.2962801722237103</v>
       </c>
       <c r="O19" t="n">
-        <v>1.803818207098438</v>
+        <v>1.7838943103090856</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -10155,46 +10148,46 @@
         <v>5</v>
       </c>
       <c r="B20" t="n">
-        <v>4.949494854731941E-6</v>
+        <v>4.945652082477192E-6</v>
       </c>
       <c r="C20" t="n">
-        <v>4.956521784063902E-6</v>
+        <v>4.960629960517049E-6</v>
       </c>
       <c r="D20" t="n">
-        <v>4.949999988730031E-6</v>
+        <v>4.943820214277601E-6</v>
       </c>
       <c r="E20" t="n">
-        <v>4.955752207552296E-6</v>
+        <v>4.954954952502122E-6</v>
       </c>
       <c r="F20" t="n">
-        <v>4.9664624364194316E-6</v>
+        <v>4.9545454558513435E-6</v>
       </c>
       <c r="G20" t="n">
-        <v>4.954545455520295E-6</v>
+        <v>4.947916667608892E-6</v>
       </c>
       <c r="H20" t="n">
-        <v>4.964870337894308E-6</v>
+        <v>4.949497035796333E-6</v>
       </c>
       <c r="I20" t="n">
-        <v>4.960333106135901E-6</v>
+        <v>4.947916666999426E-6</v>
       </c>
       <c r="J20" t="n">
-        <v>4.956405175492619E-6</v>
+        <v>5.009652555748894E-6</v>
       </c>
       <c r="K20" t="n">
-        <v>4.975134505897649E-6</v>
+        <v>4.951456310599093E-6</v>
       </c>
       <c r="L20" t="n">
-        <v>4.984150042558318E-6</v>
+        <v>4.963503682752825E-6</v>
       </c>
       <c r="M20" t="n">
-        <v>5.018532876449359E-6</v>
+        <v>4.970204118109837E-6</v>
       </c>
       <c r="N20" t="n">
-        <v>4.945538761435862E-6</v>
+        <v>4.966566743503762E-6</v>
       </c>
       <c r="O20" t="n">
-        <v>4.985714887164939E-6</v>
+        <v>4.9865391867358566E-6</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -10202,46 +10195,46 @@
         <v>6</v>
       </c>
       <c r="B21" t="n">
-        <v>2.499975165609602E-6</v>
+        <v>2.4999751780416467E-6</v>
       </c>
       <c r="C21" t="n">
-        <v>2.4999748937557025E-6</v>
+        <v>2.4999748241881353E-6</v>
       </c>
       <c r="D21" t="n">
-        <v>2.4999747233910028E-6</v>
+        <v>2.4999749029065328E-6</v>
       </c>
       <c r="E21" t="n">
-        <v>2.4999748862035987E-6</v>
+        <v>2.499975004408572E-6</v>
       </c>
       <c r="F21" t="n">
-        <v>2.4999749646274405E-6</v>
+        <v>2.4999813422027853E-6</v>
       </c>
       <c r="G21" t="n">
-        <v>2.499974960088256E-6</v>
+        <v>2.499981239594716E-6</v>
       </c>
       <c r="H21" t="n">
-        <v>2.5000111453204574E-6</v>
+        <v>2.5000037570906276E-6</v>
       </c>
       <c r="I21" t="n">
-        <v>2.499985458012544E-6</v>
+        <v>2.5000549991415243E-6</v>
       </c>
       <c r="J21" t="n">
-        <v>2.500047662200179E-6</v>
+        <v>2.5000283426746045E-6</v>
       </c>
       <c r="K21" t="n">
-        <v>2.500035881165442E-6</v>
+        <v>2.500043324880457E-6</v>
       </c>
       <c r="L21" t="n">
-        <v>2.5000404307331774E-6</v>
+        <v>2.500023400689765E-6</v>
       </c>
       <c r="M21" t="n">
-        <v>2.500070935687037E-6</v>
+        <v>2.5000148361833176E-6</v>
       </c>
       <c r="N21" t="n">
-        <v>2.5000550714419007E-6</v>
+        <v>2.5001874783697116E-6</v>
       </c>
       <c r="O21" t="n">
-        <v>2.500087642112427E-6</v>
+        <v>2.500142753698295E-6</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -10249,46 +10242,46 @@
         <v>7</v>
       </c>
       <c r="B22" t="n">
-        <v>4.0016344215596806E-5</v>
+        <v>4.001439148620459E-5</v>
       </c>
       <c r="C22" t="n">
-        <v>4.008042902772316E-5</v>
+        <v>4.007701939869165E-5</v>
       </c>
       <c r="D22" t="n">
-        <v>4.015254670999158E-5</v>
+        <v>4.015142161131034E-5</v>
       </c>
       <c r="E22" t="n">
-        <v>4.084948773161752E-5</v>
+        <v>4.08452766158973E-5</v>
       </c>
       <c r="F22" t="n">
-        <v>4.1821072855603256E-5</v>
+        <v>4.1826706500993046E-5</v>
       </c>
       <c r="G22" t="n">
-        <v>4.413891506602313E-5</v>
+        <v>4.406039778470047E-5</v>
       </c>
       <c r="H22" t="n">
-        <v>4.699489373597177E-5</v>
+        <v>4.6998366512746354E-5</v>
       </c>
       <c r="I22" t="n">
-        <v>5.0658782731821844E-5</v>
+        <v>5.0981293637326116E-5</v>
       </c>
       <c r="J22" t="n">
-        <v>5.581428292313667E-5</v>
+        <v>5.569418624363062E-5</v>
       </c>
       <c r="K22" t="n">
-        <v>6.211824940786532E-5</v>
+        <v>6.212481787561066E-5</v>
       </c>
       <c r="L22" t="n">
-        <v>7.064306645280967E-5</v>
+        <v>7.1011762666348E-5</v>
       </c>
       <c r="M22" t="n">
-        <v>8.481066996243538E-5</v>
+        <v>8.303570837280958E-5</v>
       </c>
       <c r="N22" t="n">
-        <v>1.0550178571475082E-4</v>
+        <v>1.0567963134757394E-4</v>
       </c>
       <c r="O22" t="n">
-        <v>1.4325541148922787E-4</v>
+        <v>1.4169167920419868E-4</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -10296,46 +10289,521 @@
         <v>8</v>
       </c>
       <c r="B23" t="n">
-        <v>4.0031776244610565E-5</v>
+        <v>4.00272340635286E-5</v>
       </c>
       <c r="C23" t="n">
-        <v>4.0162969713749125E-5</v>
+        <v>4.0149010333990904E-5</v>
       </c>
       <c r="D23" t="n">
-        <v>4.0285259883256785E-5</v>
+        <v>4.031623699688709E-5</v>
       </c>
       <c r="E23" t="n">
-        <v>4.1625105368083706E-5</v>
+        <v>4.162168385823553E-5</v>
       </c>
       <c r="F23" t="n">
-        <v>4.336815343301917E-5</v>
+        <v>4.334711280244024E-5</v>
       </c>
       <c r="G23" t="n">
-        <v>4.7106686392645086E-5</v>
+        <v>4.701226913237886E-5</v>
       </c>
       <c r="H23" t="n">
-        <v>5.1152927869688534E-5</v>
+        <v>5.124264792871189E-5</v>
       </c>
       <c r="I23" t="n">
-        <v>5.616491027210709E-5</v>
+        <v>5.662017023992435E-5</v>
       </c>
       <c r="J23" t="n">
-        <v>6.235933399806707E-5</v>
+        <v>6.224501776061085E-5</v>
       </c>
       <c r="K23" t="n">
-        <v>6.99194721061177E-5</v>
+        <v>6.987520502913294E-5</v>
       </c>
       <c r="L23" t="n">
-        <v>7.943978860866048E-5</v>
+        <v>7.958709809982531E-5</v>
       </c>
       <c r="M23" t="n">
-        <v>9.442829104603769E-5</v>
+        <v>9.284910416087126E-5</v>
       </c>
       <c r="N23" t="n">
-        <v>1.1615122491173048E-4</v>
+        <v>1.1625302609299373E-4</v>
       </c>
       <c r="O23" t="n">
-        <v>1.5472318207825322E-4</v>
+        <v>1.5307332857766358E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K51" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="L51" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="M51" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="N51" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="O51" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1.967016996185635E-8</v>
+      </c>
+      <c r="C52" t="n">
+        <v>9.83607057988953E-8</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1.967460571282987E-7</v>
+      </c>
+      <c r="E52" t="n">
+        <v>9.847172195223919E-7</v>
+      </c>
+      <c r="F52" t="n">
+        <v>1.9719073503224382E-6</v>
+      </c>
+      <c r="G52" t="n">
+        <v>3.9537437007605725E-6</v>
+      </c>
+      <c r="H52" t="n">
+        <v>5.945584232738673E-6</v>
+      </c>
+      <c r="I52" t="n">
+        <v>7.94750488862353E-6</v>
+      </c>
+      <c r="J52" t="n">
+        <v>9.959582381376142E-6</v>
+      </c>
+      <c r="K52" t="n">
+        <v>1.1981894204350671E-5</v>
+      </c>
+      <c r="L52" t="n">
+        <v>1.4014518641243366E-5</v>
+      </c>
+      <c r="M52" t="n">
+        <v>1.6057534776193972E-5</v>
+      </c>
+      <c r="N52" t="n">
+        <v>1.8111022504042568E-5</v>
+      </c>
+      <c r="O52" t="n">
+        <v>2.017506254074445E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" t="n">
+        <v>9.835084980928175E-6</v>
+      </c>
+      <c r="C53" t="n">
+        <v>4.9180352899447674E-5</v>
+      </c>
+      <c r="D53" t="n">
+        <v>9.837302856414932E-5</v>
+      </c>
+      <c r="E53" t="n">
+        <v>4.92358609761196E-4</v>
+      </c>
+      <c r="F53" t="n">
+        <v>9.859536751612192E-4</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.0019768718503802856</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.002972792116369337</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.003973752444311763</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.00497979119068807</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.005990947102175336</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0.007007259320621684</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0.008028767388096986</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0.009055511252021285</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0.010087531270372225</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1.5748346756022565E-4</v>
+      </c>
+      <c r="C54" t="n">
+        <v>7.899484627117246E-4</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.0015862706885188085</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.008195869590657642</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.017104810838818034</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.037469620390701515</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.06212457932506007</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.09258497146310679</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.13117488753056644</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.18164920850153596</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0.2504779584528176</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.3496092422189913</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0.5017157698429743</v>
+      </c>
+      <c r="O54" t="n">
+        <v>0.7425345550686313</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1.5764095102778583E-4</v>
+      </c>
+      <c r="C55" t="n">
+        <v>7.907384111744363E-4</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.001587856959207327</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.0082040654602483</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.017121915649656858</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.03750709001109222</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.06218670390438513</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.0926775564345699</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.131306062418097</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.18183085771003749</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0.25072843641127046</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0.3499588514612103</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0.5022174856128172</v>
+      </c>
+      <c r="O55" t="n">
+        <v>0.7432770896236998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" t="n">
+        <v>3.2499884390886337E-4</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.0016300639481972065</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.0032728941684045413</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.016894263095106183</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.035216623978336754</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.07696148973957555</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.12729596651428002</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.1892521753517657</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.26748066030411427</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.3694949771021575</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0.5082416832219923</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0.707628976137851</v>
+      </c>
+      <c r="N56" t="n">
+        <v>1.0130249887528209</v>
+      </c>
+      <c r="O56" t="n">
+        <v>1.4959395260877846</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1.967016996185635E-6</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1.967214115977906E-6</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1.9674605712829865E-6</v>
+      </c>
+      <c r="E57" t="n">
+        <v>1.9694344390447837E-6</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1.9719073503224382E-6</v>
+      </c>
+      <c r="G57" t="n">
+        <v>1.9768718503802863E-6</v>
+      </c>
+      <c r="H57" t="n">
+        <v>1.981861410912891E-6</v>
+      </c>
+      <c r="I57" t="n">
+        <v>1.9868762221558824E-6</v>
+      </c>
+      <c r="J57" t="n">
+        <v>1.9919164762752285E-6</v>
+      </c>
+      <c r="K57" t="n">
+        <v>1.9969823673917788E-6</v>
+      </c>
+      <c r="L57" t="n">
+        <v>2.0020740916061952E-6</v>
+      </c>
+      <c r="M57" t="n">
+        <v>2.0071918470242465E-6</v>
+      </c>
+      <c r="N57" t="n">
+        <v>2.0123358337825077E-6</v>
+      </c>
+      <c r="O57" t="n">
+        <v>2.0175062540744446E-6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" t="n">
+        <v>9.835084980928176E-7</v>
+      </c>
+      <c r="C58" t="n">
+        <v>9.836070579889536E-7</v>
+      </c>
+      <c r="D58" t="n">
+        <v>9.837302856414933E-7</v>
+      </c>
+      <c r="E58" t="n">
+        <v>9.847172195223919E-7</v>
+      </c>
+      <c r="F58" t="n">
+        <v>9.859536751612191E-7</v>
+      </c>
+      <c r="G58" t="n">
+        <v>9.884359251901427E-7</v>
+      </c>
+      <c r="H58" t="n">
+        <v>9.909307054564455E-7</v>
+      </c>
+      <c r="I58" t="n">
+        <v>9.934381110779408E-7</v>
+      </c>
+      <c r="J58" t="n">
+        <v>9.95958238137614E-7</v>
+      </c>
+      <c r="K58" t="n">
+        <v>9.984911836958894E-7</v>
+      </c>
+      <c r="L58" t="n">
+        <v>1.0010370458030976E-6</v>
+      </c>
+      <c r="M58" t="n">
+        <v>1.0035959235121233E-6</v>
+      </c>
+      <c r="N58" t="n">
+        <v>1.0061679168912539E-6</v>
+      </c>
+      <c r="O58" t="n">
+        <v>1.0087531270372223E-6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1.5732614141880686E-5</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1.5783186068166328E-5</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1.5846860025162923E-5</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.6375363817497784E-5</v>
+      </c>
+      <c r="F59" t="n">
+        <v>1.708772311570233E-5</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1.871609410124951E-5</v>
+      </c>
+      <c r="H59" t="n">
+        <v>2.0687505602750605E-5</v>
+      </c>
+      <c r="I59" t="n">
+        <v>2.3123119746030666E-5</v>
+      </c>
+      <c r="J59" t="n">
+        <v>2.620876873737591E-5</v>
+      </c>
+      <c r="K59" t="n">
+        <v>3.0244623460129196E-5</v>
+      </c>
+      <c r="L59" t="n">
+        <v>3.574681867458508E-5</v>
+      </c>
+      <c r="M59" t="n">
+        <v>4.365749777959432E-5</v>
+      </c>
+      <c r="N59" t="n">
+        <v>5.569050614307628E-5</v>
+      </c>
+      <c r="O59" t="n">
+        <v>7.417927623063249E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" t="n">
+        <v>3.152819020555716E-5</v>
+      </c>
+      <c r="C60" t="n">
+        <v>3.1629536446977454E-5</v>
+      </c>
+      <c r="D60" t="n">
+        <v>3.1757139184146536E-5</v>
+      </c>
+      <c r="E60" t="n">
+        <v>3.2816261840993195E-5</v>
+      </c>
+      <c r="F60" t="n">
+        <v>3.424383129931371E-5</v>
+      </c>
+      <c r="G60" t="n">
+        <v>3.7507090011092227E-5</v>
+      </c>
+      <c r="H60" t="n">
+        <v>4.145780260292343E-5</v>
+      </c>
+      <c r="I60" t="n">
+        <v>4.6338778217284955E-5</v>
+      </c>
+      <c r="J60" t="n">
+        <v>5.2522424967238804E-5</v>
+      </c>
+      <c r="K60" t="n">
+        <v>6.061028590334583E-5</v>
+      </c>
+      <c r="L60" t="n">
+        <v>7.163669611750583E-5</v>
+      </c>
+      <c r="M60" t="n">
+        <v>8.748971286530257E-5</v>
+      </c>
+      <c r="N60" t="n">
+        <v>1.1160388569173715E-4</v>
+      </c>
+      <c r="O60" t="n">
+        <v>1.4865541792473996E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>